<commit_message>
Updated excel tabular data
</commit_message>
<xml_diff>
--- a/tabular/Kuzmin-data.xlsx
+++ b/tabular/Kuzmin-data.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="NULL accessions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -2219,8 +2220,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2288,7 +2295,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2316,6 +2323,9 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2343,6 +2353,9 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2672,10 +2685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J272"/>
+  <dimension ref="A1:J270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A249" workbookViewId="0">
+      <selection activeCell="D276" sqref="D276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9853,17 +9866,20 @@
       </c>
     </row>
     <row r="236" spans="1:10">
+      <c r="A236" s="1" t="s">
+        <v>489</v>
+      </c>
       <c r="B236" s="1" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>486</v>
+        <v>82</v>
       </c>
       <c r="E236" s="1" t="s">
         <v>80</v>
       </c>
       <c r="F236" s="1">
-        <v>2003</v>
+        <v>2005</v>
       </c>
       <c r="G236" s="1" t="s">
         <v>172</v>
@@ -9879,8 +9895,11 @@
       </c>
     </row>
     <row r="237" spans="1:10">
+      <c r="A237" s="1" t="s">
+        <v>491</v>
+      </c>
       <c r="B237" s="1" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>82</v>
@@ -9889,10 +9908,10 @@
         <v>80</v>
       </c>
       <c r="F237" s="1">
-        <v>2004</v>
+        <v>1994</v>
       </c>
       <c r="G237" s="1" t="s">
-        <v>172</v>
+        <v>88</v>
       </c>
       <c r="H237" s="1" t="s">
         <v>65</v>
@@ -9906,22 +9925,22 @@
     </row>
     <row r="238" spans="1:10">
       <c r="A238" s="1" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>82</v>
+        <v>162</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F238" s="1">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G238" s="1" t="s">
-        <v>172</v>
+        <v>88</v>
       </c>
       <c r="H238" s="1" t="s">
         <v>65</v>
@@ -9935,19 +9954,19 @@
     </row>
     <row r="239" spans="1:10">
       <c r="A239" s="1" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>82</v>
+        <v>495</v>
       </c>
       <c r="E239" s="1" t="s">
         <v>80</v>
       </c>
       <c r="F239" s="1">
-        <v>1994</v>
+        <v>1999</v>
       </c>
       <c r="G239" s="1" t="s">
         <v>88</v>
@@ -9964,22 +9983,22 @@
     </row>
     <row r="240" spans="1:10">
       <c r="A240" s="1" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>162</v>
+        <v>498</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F240" s="1">
-        <v>2004</v>
+        <v>1987</v>
       </c>
       <c r="G240" s="1" t="s">
-        <v>88</v>
+        <v>458</v>
       </c>
       <c r="H240" s="1" t="s">
         <v>65</v>
@@ -9988,27 +10007,27 @@
         <v>430</v>
       </c>
       <c r="J240" s="1" t="s">
-        <v>163</v>
+        <v>450</v>
       </c>
     </row>
     <row r="241" spans="1:10">
       <c r="A241" s="1" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="E241" s="1" t="s">
         <v>80</v>
       </c>
       <c r="F241" s="1">
-        <v>1999</v>
+        <v>1985</v>
       </c>
       <c r="G241" s="1" t="s">
-        <v>88</v>
+        <v>458</v>
       </c>
       <c r="H241" s="1" t="s">
         <v>65</v>
@@ -10017,27 +10036,27 @@
         <v>430</v>
       </c>
       <c r="J241" s="1" t="s">
-        <v>163</v>
+        <v>450</v>
       </c>
     </row>
     <row r="242" spans="1:10">
       <c r="A242" s="1" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>497</v>
+        <v>503</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>498</v>
+        <v>179</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F242" s="1">
-        <v>1987</v>
+        <v>504</v>
+      </c>
+      <c r="F242" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="G242" s="1" t="s">
-        <v>458</v>
+        <v>225</v>
       </c>
       <c r="H242" s="1" t="s">
         <v>65</v>
@@ -10046,27 +10065,27 @@
         <v>430</v>
       </c>
       <c r="J242" s="1" t="s">
-        <v>450</v>
+        <v>505</v>
       </c>
     </row>
     <row r="243" spans="1:10">
       <c r="A243" s="1" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>501</v>
+        <v>179</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F243" s="1">
-        <v>1985</v>
+        <v>507</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="G243" s="1" t="s">
-        <v>458</v>
+        <v>196</v>
       </c>
       <c r="H243" s="1" t="s">
         <v>65</v>
@@ -10075,27 +10094,27 @@
         <v>430</v>
       </c>
       <c r="J243" s="1" t="s">
-        <v>450</v>
+        <v>505</v>
       </c>
     </row>
     <row r="244" spans="1:10">
       <c r="A244" s="1" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>179</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="F244" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G244" s="1" t="s">
-        <v>225</v>
+        <v>196</v>
       </c>
       <c r="H244" s="1" t="s">
         <v>65</v>
@@ -10109,10 +10128,10 @@
     </row>
     <row r="245" spans="1:10">
       <c r="A245" s="1" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>179</v>
@@ -10124,7 +10143,7 @@
         <v>65</v>
       </c>
       <c r="G245" s="1" t="s">
-        <v>196</v>
+        <v>510</v>
       </c>
       <c r="H245" s="1" t="s">
         <v>65</v>
@@ -10133,15 +10152,15 @@
         <v>430</v>
       </c>
       <c r="J245" s="1" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
     </row>
     <row r="246" spans="1:10">
       <c r="A246" s="1" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>179</v>
@@ -10152,9 +10171,6 @@
       <c r="F246" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G246" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="H246" s="1" t="s">
         <v>65</v>
       </c>
@@ -10162,21 +10178,21 @@
         <v>430</v>
       </c>
       <c r="J246" s="1" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
     </row>
     <row r="247" spans="1:10">
       <c r="A247" s="1" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>179</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="F247" s="1" t="s">
         <v>65</v>
@@ -10196,19 +10212,22 @@
     </row>
     <row r="248" spans="1:10">
       <c r="A248" s="1" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>179</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>507</v>
+        <v>516</v>
       </c>
       <c r="F248" s="1" t="s">
         <v>65</v>
+      </c>
+      <c r="G248" s="1" t="s">
+        <v>510</v>
       </c>
       <c r="H248" s="1" t="s">
         <v>65</v>
@@ -10222,16 +10241,16 @@
     </row>
     <row r="249" spans="1:10">
       <c r="A249" s="1" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>179</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="F249" s="1" t="s">
         <v>65</v>
@@ -10251,10 +10270,10 @@
     </row>
     <row r="250" spans="1:10">
       <c r="A250" s="1" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>179</v>
@@ -10280,16 +10299,16 @@
     </row>
     <row r="251" spans="1:10">
       <c r="A251" s="1" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>179</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="F251" s="1" t="s">
         <v>65</v>
@@ -10309,22 +10328,25 @@
     </row>
     <row r="252" spans="1:10">
       <c r="A252" s="1" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>179</v>
+        <v>227</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>575</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="F252" s="1" t="s">
-        <v>65</v>
+        <v>385</v>
+      </c>
+      <c r="F252" s="1">
+        <v>1981</v>
       </c>
       <c r="G252" s="1" t="s">
-        <v>510</v>
+        <v>311</v>
       </c>
       <c r="H252" s="1" t="s">
         <v>65</v>
@@ -10333,27 +10355,30 @@
         <v>430</v>
       </c>
       <c r="J252" s="1" t="s">
-        <v>511</v>
+        <v>450</v>
       </c>
     </row>
     <row r="253" spans="1:10">
       <c r="A253" s="1" t="s">
-        <v>519</v>
+        <v>524</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>179</v>
+        <v>227</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>575</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="F253" s="1" t="s">
-        <v>65</v>
+        <v>385</v>
+      </c>
+      <c r="F253" s="1">
+        <v>1982</v>
       </c>
       <c r="G253" s="1" t="s">
-        <v>510</v>
+        <v>311</v>
       </c>
       <c r="H253" s="1" t="s">
         <v>65</v>
@@ -10362,30 +10387,30 @@
         <v>430</v>
       </c>
       <c r="J253" s="1" t="s">
-        <v>511</v>
+        <v>450</v>
       </c>
     </row>
     <row r="254" spans="1:10">
       <c r="A254" s="1" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>575</v>
+        <v>552</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>385</v>
+        <v>87</v>
       </c>
       <c r="F254" s="1">
-        <v>1981</v>
+        <v>1994</v>
       </c>
       <c r="G254" s="1" t="s">
-        <v>311</v>
+        <v>186</v>
       </c>
       <c r="H254" s="1" t="s">
         <v>65</v>
@@ -10394,94 +10419,94 @@
         <v>430</v>
       </c>
       <c r="J254" s="1" t="s">
-        <v>450</v>
+        <v>526</v>
       </c>
     </row>
     <row r="255" spans="1:10">
       <c r="A255" s="1" t="s">
-        <v>524</v>
+        <v>689</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>385</v>
+        <v>17</v>
       </c>
       <c r="F255" s="1">
-        <v>1982</v>
+        <v>2010</v>
       </c>
       <c r="G255" s="1" t="s">
-        <v>311</v>
+        <v>222</v>
       </c>
       <c r="H255" s="1" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="I255" s="1" t="s">
         <v>430</v>
       </c>
       <c r="J255" s="1" t="s">
-        <v>450</v>
+        <v>9</v>
       </c>
     </row>
     <row r="256" spans="1:10">
       <c r="A256" s="1" t="s">
-        <v>525</v>
+        <v>690</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>552</v>
+        <v>577</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>87</v>
+        <v>385</v>
       </c>
       <c r="F256" s="1">
-        <v>1994</v>
+        <v>2010</v>
       </c>
       <c r="G256" s="1" t="s">
-        <v>186</v>
+        <v>311</v>
       </c>
       <c r="H256" s="1" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="I256" s="1" t="s">
         <v>430</v>
       </c>
       <c r="J256" s="1" t="s">
-        <v>526</v>
+        <v>9</v>
       </c>
     </row>
     <row r="257" spans="1:10">
       <c r="A257" s="1" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>576</v>
+        <v>552</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>17</v>
+        <v>385</v>
       </c>
       <c r="F257" s="1">
-        <v>2010</v>
+        <v>1991</v>
       </c>
       <c r="G257" s="1" t="s">
-        <v>222</v>
+        <v>311</v>
       </c>
       <c r="H257" s="1" t="s">
         <v>8</v>
@@ -10495,25 +10520,25 @@
     </row>
     <row r="258" spans="1:10">
       <c r="A258" s="1" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>577</v>
+        <v>552</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>385</v>
+        <v>195</v>
       </c>
       <c r="F258" s="1">
-        <v>2010</v>
+        <v>1994</v>
       </c>
       <c r="G258" s="1" t="s">
-        <v>311</v>
+        <v>196</v>
       </c>
       <c r="H258" s="1" t="s">
         <v>8</v>
@@ -10527,25 +10552,25 @@
     </row>
     <row r="259" spans="1:10">
       <c r="A259" s="1" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>552</v>
+        <v>578</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>385</v>
+        <v>201</v>
       </c>
       <c r="F259" s="1">
-        <v>1991</v>
+        <v>2010</v>
       </c>
       <c r="G259" s="1" t="s">
-        <v>311</v>
+        <v>202</v>
       </c>
       <c r="H259" s="1" t="s">
         <v>8</v>
@@ -10559,25 +10584,25 @@
     </row>
     <row r="260" spans="1:10">
       <c r="A260" s="1" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>552</v>
+        <v>579</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="F260" s="1">
-        <v>1994</v>
+        <v>2010</v>
       </c>
       <c r="G260" s="1" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="H260" s="1" t="s">
         <v>8</v>
@@ -10591,10 +10616,10 @@
     </row>
     <row r="261" spans="1:10">
       <c r="A261" s="1" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>227</v>
@@ -10603,13 +10628,13 @@
         <v>578</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>201</v>
+        <v>17</v>
       </c>
       <c r="F261" s="1">
         <v>2010</v>
       </c>
       <c r="G261" s="1" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="H261" s="1" t="s">
         <v>8</v>
@@ -10623,25 +10648,25 @@
     </row>
     <row r="262" spans="1:10">
       <c r="A262" s="1" t="s">
-        <v>694</v>
+        <v>535</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="F262" s="1">
         <v>2010</v>
       </c>
       <c r="G262" s="1" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="H262" s="1" t="s">
         <v>8</v>
@@ -10655,25 +10680,25 @@
     </row>
     <row r="263" spans="1:10">
       <c r="A263" s="1" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>17</v>
+        <v>185</v>
       </c>
       <c r="F263" s="1">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G263" s="1" t="s">
-        <v>212</v>
+        <v>186</v>
       </c>
       <c r="H263" s="1" t="s">
         <v>8</v>
@@ -10687,25 +10712,25 @@
     </row>
     <row r="264" spans="1:10">
       <c r="A264" s="1" t="s">
-        <v>535</v>
+        <v>697</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>578</v>
+        <v>564</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="F264" s="1">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="G264" s="1" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="H264" s="1" t="s">
         <v>8</v>
@@ -10719,25 +10744,25 @@
     </row>
     <row r="265" spans="1:10">
       <c r="A265" s="1" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>579</v>
+        <v>566</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>185</v>
+        <v>219</v>
       </c>
       <c r="F265" s="1">
-        <v>2009</v>
+        <v>1993</v>
       </c>
       <c r="G265" s="1" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="H265" s="1" t="s">
         <v>8</v>
@@ -10751,25 +10776,25 @@
     </row>
     <row r="266" spans="1:10">
       <c r="A266" s="1" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>564</v>
+        <v>578</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="F266" s="1">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="G266" s="1" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="H266" s="1" t="s">
         <v>8</v>
@@ -10783,25 +10808,25 @@
     </row>
     <row r="267" spans="1:10">
       <c r="A267" s="1" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>566</v>
+        <v>551</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>219</v>
+        <v>20</v>
       </c>
       <c r="F267" s="1">
-        <v>1993</v>
+        <v>2011</v>
       </c>
       <c r="G267" s="1" t="s">
-        <v>220</v>
+        <v>311</v>
       </c>
       <c r="H267" s="1" t="s">
         <v>8</v>
@@ -10815,25 +10840,25 @@
     </row>
     <row r="268" spans="1:10">
       <c r="A268" s="1" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>578</v>
+        <v>566</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>198</v>
+        <v>20</v>
       </c>
       <c r="F268" s="1">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="G268" s="1" t="s">
-        <v>199</v>
+        <v>311</v>
       </c>
       <c r="H268" s="1" t="s">
         <v>8</v>
@@ -10847,25 +10872,25 @@
     </row>
     <row r="269" spans="1:10">
       <c r="A269" s="1" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>551</v>
+        <v>580</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="F269" s="1">
         <v>2011</v>
       </c>
       <c r="G269" s="1" t="s">
-        <v>311</v>
+        <v>202</v>
       </c>
       <c r="H269" s="1" t="s">
         <v>8</v>
@@ -10879,25 +10904,25 @@
     </row>
     <row r="270" spans="1:10">
       <c r="A270" s="1" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>566</v>
+        <v>581</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>20</v>
+        <v>544</v>
       </c>
       <c r="F270" s="1">
         <v>2011</v>
       </c>
       <c r="G270" s="1" t="s">
-        <v>311</v>
+        <v>212</v>
       </c>
       <c r="H270" s="1" t="s">
         <v>8</v>
@@ -10906,70 +10931,6 @@
         <v>430</v>
       </c>
       <c r="J270" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="271" spans="1:10">
-      <c r="A271" s="1" t="s">
-        <v>702</v>
-      </c>
-      <c r="B271" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="C271" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D271" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="E271" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F271" s="1">
-        <v>2011</v>
-      </c>
-      <c r="G271" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="H271" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I271" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="J271" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="272" spans="1:10">
-      <c r="A272" s="1" t="s">
-        <v>703</v>
-      </c>
-      <c r="B272" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="C272" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D272" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="E272" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="F272" s="1">
-        <v>2011</v>
-      </c>
-      <c r="G272" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="H272" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I272" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="J272" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -10982,4 +10943,80 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27:G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2003</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2004</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Corrected a few incorrectly assigned genotypes
</commit_message>
<xml_diff>
--- a/tabular/Kuzmin-data.xlsx
+++ b/tabular/Kuzmin-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="0" windowWidth="23560" windowHeight="23980" tabRatio="500"/>
+    <workbookView xWindow="18360" yWindow="3040" windowWidth="23560" windowHeight="23980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Kuzmin-data.csv" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2131" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2138" uniqueCount="727">
   <si>
     <t>Year</t>
   </si>
@@ -2180,6 +2180,27 @@
   </si>
   <si>
     <t>Bat - TB</t>
+  </si>
+  <si>
+    <t>BR-NL2</t>
+  </si>
+  <si>
+    <t>BR-EF4</t>
+  </si>
+  <si>
+    <t>BR-EF3</t>
+  </si>
+  <si>
+    <t>BR-EF1</t>
+  </si>
+  <si>
+    <t>9135OMA</t>
+  </si>
+  <si>
+    <t>8706ARS</t>
+  </si>
+  <si>
+    <t>8702IRA</t>
   </si>
 </sst>
 </file>
@@ -2269,8 +2290,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="225">
+  <cellStyleXfs count="251">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2515,7 +2562,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="225">
+  <cellStyles count="251">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2628,6 +2675,19 @@
     <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2740,6 +2800,19 @@
     <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3071,8 +3144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="D53" sqref="A1:J270"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="B262" sqref="B262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3296,7 +3369,9 @@
       <c r="A10" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="B10"/>
+      <c r="B10" t="s">
+        <v>723</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>166</v>
       </c>
@@ -3317,7 +3392,9 @@
       <c r="A11" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="B11"/>
+      <c r="B11" t="s">
+        <v>722</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>166</v>
       </c>
@@ -3338,7 +3415,9 @@
       <c r="A12" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="B12"/>
+      <c r="B12" t="s">
+        <v>721</v>
+      </c>
       <c r="C12" s="1" t="s">
         <v>166</v>
       </c>
@@ -3359,7 +3438,9 @@
       <c r="A13" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="B13"/>
+      <c r="B13" t="s">
+        <v>720</v>
+      </c>
       <c r="C13" s="1" t="s">
         <v>166</v>
       </c>
@@ -4273,7 +4354,7 @@
         <v>1995</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>45</v>
@@ -10529,7 +10610,9 @@
       <c r="A260" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B260"/>
+      <c r="B260" t="s">
+        <v>724</v>
+      </c>
       <c r="C260" s="1" t="s">
         <v>122</v>
       </c>
@@ -10553,7 +10636,9 @@
       <c r="A261" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B261"/>
+      <c r="B261" t="s">
+        <v>725</v>
+      </c>
       <c r="C261" s="1" t="s">
         <v>119</v>
       </c>
@@ -10577,7 +10662,9 @@
       <c r="A262" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B262"/>
+      <c r="B262" t="s">
+        <v>726</v>
+      </c>
       <c r="C262" s="1" t="s">
         <v>125</v>
       </c>

</xml_diff>